<commit_message>
Se introduce al servidor xlsx-passport, se crea en el back de finanzas, la posibilidad de generar comprobantes de pago desde una plantilla excel.
</commit_message>
<xml_diff>
--- a/src/public/plantillas/ReciboDePago.xlsx
+++ b/src/public/plantillas/ReciboDePago.xlsx
@@ -2,21 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\ServerJoval\src\public\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB1F6DB-F6B4-4427-9C4E-8C165129D7C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E6312D-1569-4146-AA78-79E82C644831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{865199D7-FC27-416A-B732-E3AE2DDF80F3}"/>
   </bookViews>
   <sheets>
-    <sheet name="ReciboDePago" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">ReciboDePago!$B$2:$S$26</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$B$2:$S$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>LIQUIDACIÓN DE PAGO</t>
   </si>
@@ -69,6 +69,9 @@
     <t>,</t>
   </si>
   <si>
+    <t>RECIBO</t>
+  </si>
+  <si>
     <t>Percibido por los conceptos indicados al margen.</t>
   </si>
   <si>
@@ -78,6 +81,9 @@
     <t>SERVICIO DOMICILIARIO</t>
   </si>
   <si>
+    <t>PESOS TREINTA Y CINCO MIL CON 00/100,-</t>
+  </si>
+  <si>
     <t>En concepto de pago en efectivo por Servicio Domiciliario. -</t>
   </si>
   <si>
@@ -90,13 +96,10 @@
     <t>BARRIO BICENTENARIO MANZANA D; CASA 4</t>
   </si>
   <si>
-    <t>RECIBO DE PAGO</t>
-  </si>
-  <si>
-    <t>PESOS TREINTA Y CINCO MIL CON 00/100-</t>
-  </si>
-  <si>
     <t>Observaciones:</t>
+  </si>
+  <si>
+    <t>Sin observaciones</t>
   </si>
 </sst>
 </file>
@@ -108,7 +111,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,29 +207,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -432,12 +412,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -455,7 +432,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -523,6 +500,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
     </xf>
@@ -541,38 +521,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1002,13 +974,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C6E7AA5-6C1B-417D-8502-A6535DB629C7}">
-  <sheetPr codeName="Hoja1">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:S27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18:N18"/>
+      <selection activeCell="E12" sqref="E12:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,7 +995,6 @@
     <col min="13" max="13" width="3.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.85546875" customWidth="1"/>
     <col min="15" max="15" width="1.42578125" customWidth="1"/>
-    <col min="16" max="16" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="22.7109375" customWidth="1"/>
     <col min="19" max="19" width="3.5703125" customWidth="1"/>
@@ -1032,192 +1003,188 @@
   <sheetData>
     <row r="1" spans="2:19" ht="8.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:19" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="6"/>
-    </row>
-    <row r="3" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="7"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="P3" s="45" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="5"/>
+    </row>
+    <row r="3" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="P3" t="s">
         <v>10</v>
       </c>
       <c r="Q3">
         <v>1</v>
       </c>
-      <c r="S3" s="8"/>
+      <c r="S3" s="7"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="7"/>
-      <c r="S4" s="8"/>
+      <c r="B4" s="6"/>
+      <c r="S4" s="7"/>
     </row>
     <row r="5" spans="2:19" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="7"/>
-      <c r="L5" s="14" t="s">
-        <v>14</v>
+      <c r="B5" s="6"/>
+      <c r="L5" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="20">
+      <c r="N5" s="19">
         <f ca="1">+TODAY()</f>
-        <v>44922</v>
-      </c>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="8"/>
+        <v>44924</v>
+      </c>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="7"/>
     </row>
     <row r="6" spans="2:19" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="7"/>
-      <c r="C6" s="22" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="S6" s="8"/>
+        <v>14</v>
+      </c>
+      <c r="S6" s="7"/>
     </row>
     <row r="7" spans="2:19" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="7"/>
-      <c r="C7" s="21" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21" t="s">
+      <c r="D7" s="20"/>
+      <c r="E7" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="21"/>
+      <c r="F7" s="20"/>
       <c r="G7" s="38"/>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J7" s="1"/>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="8"/>
+      <c r="L7" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="7"/>
     </row>
     <row r="8" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-      <c r="C8" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="24">
+      <c r="B8" s="6"/>
+      <c r="C8" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="22"/>
+      <c r="E8" s="23">
         <v>35000</v>
       </c>
-      <c r="F8" s="24"/>
+      <c r="F8" s="23"/>
       <c r="G8" s="38"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="27"/>
-      <c r="S8" s="8"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="26"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="26"/>
+      <c r="S8" s="7"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="38"/>
-      <c r="I9" s="29" t="s">
+      <c r="I9" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="8"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="7"/>
     </row>
     <row r="10" spans="2:19" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="17"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="16"/>
       <c r="G10" s="38"/>
-      <c r="S10" s="8"/>
+      <c r="S10" s="7"/>
     </row>
     <row r="11" spans="2:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="7"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="19"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="18"/>
       <c r="G11" s="38"/>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="28"/>
-      <c r="P11" s="28"/>
-      <c r="Q11" s="28"/>
-      <c r="R11" s="28"/>
-      <c r="S11" s="8"/>
+      <c r="J11" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27"/>
+      <c r="S11" s="7"/>
     </row>
     <row r="12" spans="2:19" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="17"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="16"/>
       <c r="G12" s="38"/>
       <c r="I12" s="43"/>
       <c r="J12" s="43"/>
@@ -1229,88 +1196,78 @@
       <c r="P12" s="43"/>
       <c r="Q12" s="43"/>
       <c r="R12" s="43"/>
-      <c r="S12" s="8"/>
+      <c r="S12" s="7"/>
     </row>
     <row r="13" spans="2:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="7"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="19"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="18"/>
       <c r="G13" s="38"/>
-      <c r="I13" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="36"/>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36"/>
-      <c r="M13" s="36"/>
-      <c r="N13" s="36"/>
-      <c r="O13" s="36"/>
-      <c r="P13" s="36"/>
-      <c r="Q13" s="36"/>
-      <c r="R13" s="36"/>
-      <c r="S13" s="8"/>
+      <c r="I13" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="35"/>
+      <c r="P13" s="35"/>
+      <c r="Q13" s="35"/>
+      <c r="R13" s="35"/>
+      <c r="S13" s="7"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="17"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="16"/>
       <c r="G14" s="38"/>
-      <c r="S14" s="8"/>
-    </row>
-    <row r="15" spans="2:19" ht="21" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="19"/>
+      <c r="S14" s="7"/>
+    </row>
+    <row r="15" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="6"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="18"/>
       <c r="G15" s="38"/>
-      <c r="I15" s="55" t="s">
+      <c r="I15" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="55"/>
-      <c r="K15" s="55"/>
-      <c r="L15" s="55"/>
-      <c r="M15" s="55"/>
-      <c r="N15" s="55"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="8"/>
-    </row>
-    <row r="16" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="P15" s="44">
+        <f>E8</f>
+        <v>35000</v>
+      </c>
+      <c r="Q15" s="44"/>
+      <c r="R15" s="44"/>
+      <c r="S15" s="7"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="16"/>
       <c r="G16" s="38"/>
-      <c r="I16" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="54"/>
-      <c r="N16" s="54"/>
-      <c r="P16" s="53">
-        <f>+$E$23</f>
-        <v>35000</v>
-      </c>
-      <c r="Q16" s="53"/>
-      <c r="R16" s="53"/>
-      <c r="S16" s="8"/>
+      <c r="S16" s="7"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="19"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="18"/>
       <c r="G17" s="38"/>
       <c r="I17" s="46"/>
       <c r="J17" s="47"/>
@@ -1318,42 +1275,46 @@
       <c r="L17" s="47"/>
       <c r="M17" s="46"/>
       <c r="N17" s="48"/>
-      <c r="P17" s="52"/>
-      <c r="Q17" s="52"/>
-      <c r="R17" s="52"/>
-      <c r="S17" s="8"/>
+      <c r="O17" s="45"/>
+      <c r="P17" s="49"/>
+      <c r="Q17" s="49"/>
+      <c r="R17" s="49"/>
+      <c r="S17" s="7"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="31" t="s">
+      <c r="B18" s="6"/>
+      <c r="C18" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="31"/>
-      <c r="E18" s="24">
+      <c r="D18" s="30"/>
+      <c r="E18" s="23">
         <f>+SUM(E8:F17)</f>
         <v>35000</v>
       </c>
-      <c r="F18" s="24"/>
+      <c r="F18" s="23"/>
       <c r="G18" s="38"/>
-      <c r="I18" s="49" t="s">
+      <c r="I18" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="J18" s="57"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="56"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="56"/>
-      <c r="P18" s="49"/>
-      <c r="Q18" s="49"/>
-      <c r="R18" s="49"/>
-      <c r="S18" s="8"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="L18" s="53"/>
+      <c r="M18" s="53"/>
+      <c r="N18" s="53"/>
+      <c r="O18" s="53"/>
+      <c r="P18" s="53"/>
+      <c r="Q18" s="53"/>
+      <c r="R18" s="53"/>
+      <c r="S18" s="7"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
       <c r="G19" s="38"/>
       <c r="I19" s="46"/>
       <c r="J19" s="50"/>
@@ -1361,35 +1322,37 @@
       <c r="L19" s="50"/>
       <c r="M19" s="46"/>
       <c r="N19" s="48"/>
-      <c r="P19" s="52"/>
-      <c r="Q19" s="52"/>
-      <c r="R19" s="52"/>
-      <c r="S19" s="8"/>
+      <c r="O19" s="45"/>
+      <c r="P19" s="49"/>
+      <c r="Q19" s="49"/>
+      <c r="R19" s="49"/>
+      <c r="S19" s="7"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
       <c r="G20" s="38"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="49"/>
-      <c r="M20" s="49"/>
-      <c r="N20" s="49"/>
-      <c r="P20" s="49"/>
-      <c r="Q20" s="49"/>
-      <c r="R20" s="49"/>
-      <c r="S20" s="8"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="45"/>
+      <c r="M20" s="45"/>
+      <c r="N20" s="45"/>
+      <c r="O20" s="45"/>
+      <c r="P20" s="45"/>
+      <c r="Q20" s="45"/>
+      <c r="R20" s="45"/>
+      <c r="S20" s="7"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B21" s="7"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
       <c r="G21" s="38"/>
       <c r="I21" s="46"/>
       <c r="J21" s="51"/>
@@ -1397,54 +1360,54 @@
       <c r="L21" s="51"/>
       <c r="M21" s="51"/>
       <c r="N21" s="51"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="52"/>
-      <c r="Q21" s="52"/>
-      <c r="R21" s="52"/>
-      <c r="S21" s="8"/>
+      <c r="O21" s="52"/>
+      <c r="P21" s="49"/>
+      <c r="Q21" s="49"/>
+      <c r="R21" s="49"/>
+      <c r="S21" s="7"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
+      <c r="B22" s="6"/>
       <c r="G22" s="38"/>
-      <c r="S22" s="8"/>
+      <c r="S22" s="7"/>
     </row>
     <row r="23" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-      <c r="C23" s="33" t="s">
+      <c r="B23" s="6"/>
+      <c r="C23" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="33"/>
-      <c r="E23" s="34">
+      <c r="D23" s="32"/>
+      <c r="E23" s="33">
         <f>SUM(E18:F21)</f>
         <v>35000</v>
       </c>
-      <c r="F23" s="34"/>
+      <c r="F23" s="33"/>
       <c r="G23" s="38"/>
-      <c r="S23" s="8"/>
+      <c r="S23" s="7"/>
     </row>
     <row r="24" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
       <c r="G24" s="38"/>
       <c r="P24" s="40" t="s">
         <v>4</v>
       </c>
       <c r="Q24" s="41">
-        <f>P19+P17+P16+P13</f>
+        <f>P19+P17+P15+P13</f>
         <v>35000</v>
       </c>
       <c r="R24" s="41"/>
-      <c r="S24" s="8"/>
+      <c r="S24" s="7"/>
     </row>
     <row r="25" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
       <c r="G25" s="38"/>
       <c r="I25" s="39" t="s">
         <v>11</v>
@@ -1454,52 +1417,51 @@
       <c r="L25" s="39"/>
       <c r="M25" s="39"/>
       <c r="N25" s="39"/>
-      <c r="O25" s="10"/>
+      <c r="O25" s="9"/>
       <c r="P25" s="40"/>
       <c r="Q25" s="42"/>
       <c r="R25" s="42"/>
-      <c r="S25" s="8"/>
+      <c r="S25" s="7"/>
     </row>
     <row r="26" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="11"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
-      <c r="O26" s="12"/>
-      <c r="P26" s="12"/>
-      <c r="Q26" s="12"/>
-      <c r="R26" s="12"/>
-      <c r="S26" s="13"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="12"/>
     </row>
     <row r="27" spans="2:19" ht="8.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="43">
-    <mergeCell ref="G2:M3"/>
-    <mergeCell ref="I16:N16"/>
-    <mergeCell ref="I15:N15"/>
-    <mergeCell ref="K18:N18"/>
+  <mergeCells count="42">
     <mergeCell ref="I13:R13"/>
+    <mergeCell ref="G2:I3"/>
     <mergeCell ref="G6:G25"/>
     <mergeCell ref="I25:N25"/>
     <mergeCell ref="P24:P25"/>
     <mergeCell ref="Q24:R25"/>
     <mergeCell ref="J21:N21"/>
     <mergeCell ref="P21:R21"/>
+    <mergeCell ref="I15:M15"/>
     <mergeCell ref="I12:R12"/>
     <mergeCell ref="J17:L17"/>
     <mergeCell ref="P19:R19"/>
     <mergeCell ref="P17:R17"/>
-    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="P15:R15"/>
     <mergeCell ref="J19:L19"/>
+    <mergeCell ref="K18:R18"/>
     <mergeCell ref="C18:D19"/>
     <mergeCell ref="E18:F19"/>
     <mergeCell ref="C20:D21"/>

</xml_diff>

<commit_message>
ediciones en recibo de pago y en como se carga el mismo.
</commit_message>
<xml_diff>
--- a/src/public/plantillas/ReciboDePago.xlsx
+++ b/src/public/plantillas/ReciboDePago.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\ServerJoval\src\public\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E6312D-1569-4146-AA78-79E82C644831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E31631-64FF-4CF5-A5A0-142F5AB2BD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{865199D7-FC27-416A-B732-E3AE2DDF80F3}"/>
   </bookViews>
@@ -78,28 +78,28 @@
     <t>Mendoza</t>
   </si>
   <si>
-    <t>SERVICIO DOMICILIARIO</t>
-  </si>
-  <si>
-    <t>PESOS TREINTA Y CINCO MIL CON 00/100,-</t>
-  </si>
-  <si>
-    <t>En concepto de pago en efectivo por Servicio Domiciliario. -</t>
-  </si>
-  <si>
     <t>Trasferencia bancaria por</t>
   </si>
   <si>
-    <t>SOSA GABRIEL A.</t>
-  </si>
-  <si>
-    <t>BARRIO BICENTENARIO MANZANA D; CASA 4</t>
-  </si>
-  <si>
     <t>Observaciones:</t>
   </si>
   <si>
-    <t>Sin observaciones</t>
+    <t>SR N</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIEN PESOS </t>
+  </si>
+  <si>
+    <t>PRUEBA DE EMISION DE COMPROBANTE</t>
+  </si>
+  <si>
+    <t>Cuota2</t>
+  </si>
+  <si>
+    <t>En concepto de pago en efectivo por Cuota2</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -434,6 +434,76 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -458,9 +528,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -473,77 +540,8 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="9" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -980,7 +978,7 @@
   <dimension ref="B1:S27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:F13"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,7 +993,7 @@
     <col min="13" max="13" width="3.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.85546875" customWidth="1"/>
     <col min="15" max="15" width="1.42578125" customWidth="1"/>
-    <col min="17" max="17" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" customWidth="1"/>
     <col min="18" max="18" width="22.7109375" customWidth="1"/>
     <col min="19" max="19" width="3.5703125" customWidth="1"/>
     <col min="20" max="20" width="1.85546875" customWidth="1"/>
@@ -1008,11 +1006,11 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
@@ -1026,14 +1024,14 @@
     </row>
     <row r="3" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
       <c r="P3" t="s">
         <v>10</v>
       </c>
       <c r="Q3">
-        <v>1</v>
+        <v>229</v>
       </c>
       <c r="S3" s="7"/>
     </row>
@@ -1049,40 +1047,40 @@
       <c r="M5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="19">
+      <c r="N5" s="43">
         <f ca="1">+TODAY()</f>
-        <v>44924</v>
-      </c>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
-      <c r="Q5" s="19"/>
-      <c r="R5" s="19"/>
+        <v>45240</v>
+      </c>
+      <c r="O5" s="43"/>
+      <c r="P5" s="43"/>
+      <c r="Q5" s="43"/>
+      <c r="R5" s="43"/>
       <c r="S5" s="7"/>
     </row>
     <row r="6" spans="2:19" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="6"/>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="38" t="s">
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="21" t="s">
         <v>14</v>
       </c>
       <c r="S6" s="7"/>
     </row>
     <row r="7" spans="2:19" ht="20.25" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20" t="s">
+      <c r="D7" s="44"/>
+      <c r="E7" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="38"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="21"/>
       <c r="I7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1090,151 +1088,151 @@
       <c r="K7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="24"/>
+      <c r="L7" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" s="47"/>
+      <c r="N7" s="47"/>
+      <c r="O7" s="47"/>
+      <c r="P7" s="47"/>
+      <c r="Q7" s="47"/>
+      <c r="R7" s="47"/>
       <c r="S7" s="7"/>
     </row>
     <row r="8" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
-      <c r="C8" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="23">
-        <v>35000</v>
-      </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="38"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="26"/>
-      <c r="R8" s="26"/>
+      <c r="C8" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="46"/>
+      <c r="E8" s="35">
+        <v>100</v>
+      </c>
+      <c r="F8" s="35"/>
+      <c r="G8" s="21"/>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49"/>
       <c r="S8" s="7"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="38"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="21"/>
       <c r="I9" s="28" t="s">
         <v>7</v>
       </c>
       <c r="J9" s="28"/>
       <c r="K9" s="28"/>
-      <c r="L9" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
+      <c r="L9" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="51"/>
+      <c r="N9" s="51"/>
+      <c r="O9" s="51"/>
+      <c r="P9" s="51"/>
+      <c r="Q9" s="51"/>
+      <c r="R9" s="51"/>
       <c r="S9" s="7"/>
     </row>
     <row r="10" spans="2:19" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="38"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="21"/>
       <c r="S10" s="7"/>
     </row>
     <row r="11" spans="2:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="38"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="21"/>
       <c r="I11" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="27"/>
+      <c r="J11" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="50"/>
+      <c r="P11" s="50"/>
+      <c r="Q11" s="50"/>
+      <c r="R11" s="50"/>
       <c r="S11" s="7"/>
     </row>
     <row r="12" spans="2:19" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="6"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="38"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="43"/>
-      <c r="Q12" s="43"/>
-      <c r="R12" s="43"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="21"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="29"/>
       <c r="S12" s="7"/>
     </row>
     <row r="13" spans="2:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="38"/>
-      <c r="I13" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="35"/>
-      <c r="R13" s="35"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="21"/>
+      <c r="I13" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
       <c r="S13" s="7"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="38"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="21"/>
       <c r="S14" s="7"/>
     </row>
     <row r="15" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="38"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="21"/>
       <c r="I15" s="28" t="s">
         <v>9</v>
       </c>
@@ -1243,184 +1241,170 @@
       <c r="L15" s="28"/>
       <c r="M15" s="28"/>
       <c r="N15" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="P15" s="44">
-        <f>E8</f>
-        <v>35000</v>
-      </c>
-      <c r="Q15" s="44"/>
-      <c r="R15" s="44"/>
+        <v>16</v>
+      </c>
+      <c r="P15" s="31">
+        <v>100</v>
+      </c>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="31"/>
       <c r="S15" s="7"/>
     </row>
     <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="38"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="21"/>
       <c r="S16" s="7"/>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="38"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="47"/>
-      <c r="K17" s="47"/>
-      <c r="L17" s="47"/>
-      <c r="M17" s="46"/>
-      <c r="N17" s="48"/>
-      <c r="O17" s="45"/>
-      <c r="P17" s="49"/>
-      <c r="Q17" s="49"/>
-      <c r="R17" s="49"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="21"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="15"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="27"/>
+      <c r="R17" s="27"/>
       <c r="S17" s="7"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="D18" s="30"/>
-      <c r="E18" s="23">
+      <c r="D18" s="34"/>
+      <c r="E18" s="35">
         <f>+SUM(E8:F17)</f>
-        <v>35000</v>
-      </c>
-      <c r="F18" s="23"/>
-      <c r="G18" s="38"/>
-      <c r="I18" s="45" t="s">
-        <v>22</v>
-      </c>
-      <c r="J18" s="45"/>
-      <c r="K18" s="53" t="s">
-        <v>23</v>
-      </c>
-      <c r="L18" s="53"/>
-      <c r="M18" s="53"/>
-      <c r="N18" s="53"/>
-      <c r="O18" s="53"/>
-      <c r="P18" s="53"/>
-      <c r="Q18" s="53"/>
-      <c r="R18" s="53"/>
+        <v>100</v>
+      </c>
+      <c r="F18" s="35"/>
+      <c r="G18" s="21"/>
+      <c r="I18" t="s">
+        <v>17</v>
+      </c>
+      <c r="K18" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="33"/>
+      <c r="P18" s="33"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="33"/>
       <c r="S18" s="7"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="38"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="50"/>
-      <c r="K19" s="50"/>
-      <c r="L19" s="50"/>
-      <c r="M19" s="46"/>
-      <c r="N19" s="48"/>
-      <c r="O19" s="45"/>
-      <c r="P19" s="49"/>
-      <c r="Q19" s="49"/>
-      <c r="R19" s="49"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="21"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="15"/>
+      <c r="P19" s="27"/>
+      <c r="Q19" s="27"/>
+      <c r="R19" s="27"/>
       <c r="S19" s="7"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="38"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="45"/>
-      <c r="P20" s="45"/>
-      <c r="Q20" s="45"/>
-      <c r="R20" s="45"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="21"/>
       <c r="S20" s="7"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="38"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="51"/>
-      <c r="M21" s="51"/>
-      <c r="N21" s="51"/>
-      <c r="O21" s="52"/>
-      <c r="P21" s="49"/>
-      <c r="Q21" s="49"/>
-      <c r="R21" s="49"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="21"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="27"/>
       <c r="S21" s="7"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
-      <c r="G22" s="38"/>
+      <c r="G22" s="21"/>
       <c r="S22" s="7"/>
     </row>
     <row r="23" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="32"/>
-      <c r="E23" s="33">
+      <c r="D23" s="37"/>
+      <c r="E23" s="38">
         <f>SUM(E18:F21)</f>
-        <v>35000</v>
-      </c>
-      <c r="F23" s="33"/>
-      <c r="G23" s="38"/>
+        <v>100</v>
+      </c>
+      <c r="F23" s="38"/>
+      <c r="G23" s="21"/>
       <c r="S23" s="7"/>
     </row>
     <row r="24" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="38"/>
-      <c r="P24" s="40" t="s">
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="21"/>
+      <c r="P24" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="Q24" s="41">
+      <c r="Q24" s="24">
         <f>P19+P17+P15+P13</f>
-        <v>35000</v>
-      </c>
-      <c r="R24" s="41"/>
+        <v>100</v>
+      </c>
+      <c r="R24" s="24"/>
       <c r="S24" s="7"/>
     </row>
     <row r="25" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="6"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="38"/>
-      <c r="I25" s="39" t="s">
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="21"/>
+      <c r="I25" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="39"/>
-      <c r="N25" s="39"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
       <c r="O25" s="9"/>
-      <c r="P25" s="40"/>
-      <c r="Q25" s="42"/>
-      <c r="R25" s="42"/>
+      <c r="P25" s="23"/>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="25"/>
       <c r="S25" s="7"/>
     </row>
     <row r="26" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1446,6 +1430,32 @@
     <row r="27" spans="2:19" ht="8.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="C10:D11"/>
+    <mergeCell ref="E10:F11"/>
+    <mergeCell ref="N5:R5"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C8:D9"/>
+    <mergeCell ref="E8:F9"/>
+    <mergeCell ref="L7:R7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="L8:R8"/>
+    <mergeCell ref="J11:R11"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="L9:R9"/>
+    <mergeCell ref="C12:D13"/>
+    <mergeCell ref="E12:F13"/>
+    <mergeCell ref="C14:D15"/>
+    <mergeCell ref="E14:F15"/>
+    <mergeCell ref="C16:D17"/>
+    <mergeCell ref="E16:F17"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="C20:D21"/>
+    <mergeCell ref="E20:F21"/>
+    <mergeCell ref="C23:D25"/>
+    <mergeCell ref="E23:F25"/>
     <mergeCell ref="I13:R13"/>
     <mergeCell ref="G2:I3"/>
     <mergeCell ref="G6:G25"/>
@@ -1462,32 +1472,6 @@
     <mergeCell ref="P15:R15"/>
     <mergeCell ref="J19:L19"/>
     <mergeCell ref="K18:R18"/>
-    <mergeCell ref="C18:D19"/>
-    <mergeCell ref="E18:F19"/>
-    <mergeCell ref="C20:D21"/>
-    <mergeCell ref="E20:F21"/>
-    <mergeCell ref="C23:D25"/>
-    <mergeCell ref="E23:F25"/>
-    <mergeCell ref="C12:D13"/>
-    <mergeCell ref="E12:F13"/>
-    <mergeCell ref="C14:D15"/>
-    <mergeCell ref="E14:F15"/>
-    <mergeCell ref="C16:D17"/>
-    <mergeCell ref="E16:F17"/>
-    <mergeCell ref="C10:D11"/>
-    <mergeCell ref="E10:F11"/>
-    <mergeCell ref="N5:R5"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C8:D9"/>
-    <mergeCell ref="E8:F9"/>
-    <mergeCell ref="L7:R7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="L8:R8"/>
-    <mergeCell ref="J11:R11"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="L9:R9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="121" scale="80" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
ahora el comprobante de pago sale con el nombre de archivo
</commit_message>
<xml_diff>
--- a/src/public/plantillas/ReciboDePago.xlsx
+++ b/src/public/plantillas/ReciboDePago.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E31631-64FF-4CF5-A5A0-142F5AB2BD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{865199D7-FC27-416A-B732-E3AE2DDF80F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{865199D7-FC27-416A-B732-E3AE2DDF80F3}" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t>LIQUIDACIÓN DE PAGO</t>
   </si>
@@ -100,18 +100,54 @@
   </si>
   <si>
     <t>En concepto de pago en efectivo por Cuota2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALVAREZ MARIA ALISA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuota1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UN PESO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">En concepto de pago en efectivo por Cuota1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transferencia bancaria por:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transf n°:0|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Efectivo por:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,7 +244,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills>
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,7 +258,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders>
     <border>
       <left/>
       <right/>
@@ -412,7 +448,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -975,7 +1011,6 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:S27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="N15" sqref="N15"/>
@@ -1006,7 +1041,7 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="19" t="s">
+      <c r="G2" t="s" s="19">
         <v>13</v>
       </c>
       <c r="H2" s="19"/>
@@ -1030,9 +1065,7 @@
       <c r="P3" t="s">
         <v>10</v>
       </c>
-      <c r="Q3">
-        <v>229</v>
-      </c>
+      <c r="Q3"/>
       <c r="S3" s="7"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.25">
@@ -1041,15 +1074,14 @@
     </row>
     <row r="5" spans="2:19" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B5" s="6"/>
-      <c r="L5" s="13" t="s">
+      <c r="L5" t="s" s="13">
         <v>15</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" t="s" s="1">
         <v>12</v>
       </c>
       <c r="N5" s="43">
         <f ca="1">+TODAY()</f>
-        <v>45240</v>
       </c>
       <c r="O5" s="43"/>
       <c r="P5" s="43"/>
@@ -1059,37 +1091,37 @@
     </row>
     <row r="6" spans="2:19" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="6"/>
-      <c r="C6" s="45" t="s">
+      <c r="C6" t="s" s="45">
         <v>0</v>
       </c>
       <c r="D6" s="45"/>
       <c r="E6" s="45"/>
       <c r="F6" s="45"/>
-      <c r="G6" s="21" t="s">
+      <c r="G6" t="s" s="21">
         <v>14</v>
       </c>
       <c r="S6" s="7"/>
     </row>
     <row r="7" spans="2:19" ht="20.25" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
-      <c r="C7" s="44" t="s">
+      <c r="C7" t="s" s="44">
         <v>1</v>
       </c>
       <c r="D7" s="44"/>
-      <c r="E7" s="44" t="s">
+      <c r="E7" t="s" s="44">
         <v>2</v>
       </c>
       <c r="F7" s="44"/>
       <c r="G7" s="21"/>
-      <c r="I7" s="2" t="s">
+      <c r="I7" t="s" s="2">
         <v>5</v>
       </c>
       <c r="J7" s="1"/>
-      <c r="K7" s="2" t="s">
+      <c r="K7" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="L7" s="47" t="s">
-        <v>18</v>
+      <c r="L7" t="s" s="47">
+        <v>24</v>
       </c>
       <c r="M7" s="47"/>
       <c r="N7" s="47"/>
@@ -1101,12 +1133,12 @@
     </row>
     <row r="8" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
-      <c r="C8" s="46" t="s">
-        <v>22</v>
+      <c r="C8" t="s" s="46">
+        <v>25</v>
       </c>
       <c r="D8" s="46"/>
       <c r="E8" s="35">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F8" s="35"/>
       <c r="G8" s="21"/>
@@ -1129,13 +1161,13 @@
       <c r="E9" s="35"/>
       <c r="F9" s="35"/>
       <c r="G9" s="21"/>
-      <c r="I9" s="28" t="s">
+      <c r="I9" t="s" s="28">
         <v>7</v>
       </c>
       <c r="J9" s="28"/>
       <c r="K9" s="28"/>
-      <c r="L9" s="51" t="s">
-        <v>19</v>
+      <c r="L9" t="s" s="51">
+        <v>26</v>
       </c>
       <c r="M9" s="51"/>
       <c r="N9" s="51"/>
@@ -1161,11 +1193,11 @@
       <c r="E11" s="41"/>
       <c r="F11" s="42"/>
       <c r="G11" s="21"/>
-      <c r="I11" s="8" t="s">
+      <c r="I11" t="s" s="8">
         <v>8</v>
       </c>
-      <c r="J11" s="50" t="s">
-        <v>20</v>
+      <c r="J11" t="s" s="50">
+        <v>27</v>
       </c>
       <c r="K11" s="50"/>
       <c r="L11" s="50"/>
@@ -1203,8 +1235,8 @@
       <c r="E13" s="41"/>
       <c r="F13" s="42"/>
       <c r="G13" s="21"/>
-      <c r="I13" s="17" t="s">
-        <v>23</v>
+      <c r="I13" t="s" s="17">
+        <v>28</v>
       </c>
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
@@ -1233,18 +1265,18 @@
       <c r="E15" s="41"/>
       <c r="F15" s="42"/>
       <c r="G15" s="21"/>
-      <c r="I15" s="28" t="s">
+      <c r="I15" t="s" s="28">
         <v>9</v>
       </c>
       <c r="J15" s="28"/>
       <c r="K15" s="28"/>
       <c r="L15" s="28"/>
       <c r="M15" s="28"/>
-      <c r="N15" s="14" t="s">
-        <v>16</v>
+      <c r="N15" t="s" s="14">
+        <v>31</v>
       </c>
       <c r="P15" s="31">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="Q15" s="31"/>
       <c r="R15" s="31"/>
@@ -1279,21 +1311,20 @@
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
-      <c r="C18" s="34" t="s">
+      <c r="C18" t="s" s="34">
         <v>3</v>
       </c>
       <c r="D18" s="34"/>
       <c r="E18" s="35">
         <f>+SUM(E8:F17)</f>
-        <v>100</v>
       </c>
       <c r="F18" s="35"/>
       <c r="G18" s="21"/>
       <c r="I18" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="33" t="s">
-        <v>21</v>
+      <c r="K18" t="s" s="33">
+        <v>35</v>
       </c>
       <c r="L18" s="33"/>
       <c r="M18" s="33"/>
@@ -1357,13 +1388,12 @@
     </row>
     <row r="23" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
-      <c r="C23" s="37" t="s">
+      <c r="C23" t="s" s="37">
         <v>4</v>
       </c>
       <c r="D23" s="37"/>
       <c r="E23" s="38">
         <f>SUM(E18:F21)</f>
-        <v>100</v>
       </c>
       <c r="F23" s="38"/>
       <c r="G23" s="21"/>
@@ -1376,12 +1406,11 @@
       <c r="E24" s="38"/>
       <c r="F24" s="38"/>
       <c r="G24" s="21"/>
-      <c r="P24" s="23" t="s">
+      <c r="P24" t="s" s="23">
         <v>4</v>
       </c>
       <c r="Q24" s="24">
         <f>P19+P17+P15+P13</f>
-        <v>100</v>
       </c>
       <c r="R24" s="24"/>
       <c r="S24" s="7"/>
@@ -1393,7 +1422,7 @@
       <c r="E25" s="38"/>
       <c r="F25" s="38"/>
       <c r="G25" s="21"/>
-      <c r="I25" s="22" t="s">
+      <c r="I25" t="s" s="22">
         <v>11</v>
       </c>
       <c r="J25" s="22"/>

</xml_diff>

<commit_message>
ahora se carga el dni en el comprobante de pago
</commit_message>
<xml_diff>
--- a/src/public/plantillas/ReciboDePago.xlsx
+++ b/src/public/plantillas/ReciboDePago.xlsx
@@ -148,6 +148,48 @@
   </si>
   <si>
     <t xml:space="preserve">Transf n°:345|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N°:237</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CASTRO ROSANA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AnticipoFinanciero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIENTO CINCUENTA Y TRES MIL TRESCIENTOS NOVENTA Y OCHO PESOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">En concepto de pago en efectivo por AnticipoFinanciero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transf n°:123 | adgSDaS 123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N°:undefined</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALVAREZ MARIA ALISA , DNI 33051226</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">N°:239</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">N°:240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdasd</t>
   </si>
 </sst>
 </file>
@@ -1075,7 +1117,7 @@
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
       <c r="P3" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="Q3"/>
       <c r="S3" s="7"/>
@@ -1133,7 +1175,7 @@
         <v>6</v>
       </c>
       <c r="L7" t="s" s="47">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="M7" s="47"/>
       <c r="N7" s="47"/>
@@ -1285,7 +1327,7 @@
       <c r="L15" s="28"/>
       <c r="M15" s="28"/>
       <c r="N15" t="s" s="14">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="P15" s="31">
         <v>1</v>
@@ -1336,7 +1378,7 @@
         <v>17</v>
       </c>
       <c r="K18" t="s" s="33">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="L18" s="33"/>
       <c r="M18" s="33"/>

</xml_diff>

<commit_message>
se agrega descripcion cuando resta por pagar
</commit_message>
<xml_diff>
--- a/src/public/plantillas/ReciboDePago.xlsx
+++ b/src/public/plantillas/ReciboDePago.xlsx
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t xml:space="preserve">Transf n°:262637 | la la la</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
   </si>
   <si>
     <t xml:space="preserve"/>
@@ -1402,7 +1405,7 @@
         <v>17</v>
       </c>
       <c r="K18" t="s" s="33">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="L18" s="33"/>
       <c r="M18" s="33"/>

</xml_diff>

<commit_message>
correcciones en la generacion de comprobantes
</commit_message>
<xml_diff>
--- a/src/public/plantillas/ReciboDePago.xlsx
+++ b/src/public/plantillas/ReciboDePago.xlsx
@@ -217,6 +217,36 @@
   </si>
   <si>
     <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">CALDERON MARIANO , DNI 23180320</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRESCIENTOS TREINTA Y TRES PESOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">asdqasdad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N°:246</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALIRI PICON DIEGO , DNI 30819184</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UN MIL CIENTO ONCE PESOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">asd1235asdf</t>
   </si>
 </sst>
 </file>
@@ -1144,7 +1174,7 @@
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
       <c r="P3" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="Q3"/>
       <c r="S3" s="7"/>
@@ -1202,7 +1232,7 @@
         <v>6</v>
       </c>
       <c r="L7" t="s" s="47">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="M7" s="47"/>
       <c r="N7" s="47"/>
@@ -1219,7 +1249,7 @@
       </c>
       <c r="D8" s="46"/>
       <c r="E8" s="35">
-        <v>1</v>
+        <v>1111</v>
       </c>
       <c r="F8" s="35"/>
       <c r="G8" s="21"/>
@@ -1248,7 +1278,7 @@
       <c r="J9" s="28"/>
       <c r="K9" s="28"/>
       <c r="L9" t="s" s="51">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="M9" s="51"/>
       <c r="N9" s="51"/>
@@ -1278,7 +1308,7 @@
         <v>8</v>
       </c>
       <c r="J11" t="s" s="50">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="K11" s="50"/>
       <c r="L11" s="50"/>
@@ -1357,7 +1387,7 @@
         <v>31</v>
       </c>
       <c r="P15" s="31">
-        <v>1</v>
+        <v>1111</v>
       </c>
       <c r="Q15" s="31"/>
       <c r="R15" s="31"/>
@@ -1405,7 +1435,7 @@
         <v>17</v>
       </c>
       <c r="K18" t="s" s="33">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="L18" s="33"/>
       <c r="M18" s="33"/>

</xml_diff>

<commit_message>
correccion en la generacion de comprobante
</commit_message>
<xml_diff>
--- a/src/public/plantillas/ReciboDePago.xlsx
+++ b/src/public/plantillas/ReciboDePago.xlsx
@@ -268,6 +268,18 @@
   </si>
   <si>
     <t xml:space="preserve">SR N , DNI 111</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">N°:266</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">N°:267</t>
   </si>
   <si>
     <t xml:space="preserve"/>
@@ -1198,7 +1210,7 @@
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
       <c r="P3" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="Q3"/>
       <c r="S3" s="7"/>
@@ -1256,7 +1268,7 @@
         <v>6</v>
       </c>
       <c r="L7" t="s" s="47">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="M7" s="47"/>
       <c r="N7" s="47"/>
@@ -1269,7 +1281,7 @@
     <row r="8" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="C8" t="s" s="46">
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="D8" s="46"/>
       <c r="E8" s="35">
@@ -1302,7 +1314,7 @@
       <c r="J9" s="28"/>
       <c r="K9" s="28"/>
       <c r="L9" t="s" s="51">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="M9" s="51"/>
       <c r="N9" s="51"/>
@@ -1371,7 +1383,7 @@
       <c r="F13" s="42"/>
       <c r="G13" s="21"/>
       <c r="I13" t="s" s="17">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="J13" s="18"/>
       <c r="K13" s="18"/>
@@ -1459,7 +1471,7 @@
         <v>17</v>
       </c>
       <c r="K18" t="s" s="33">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="L18" s="33"/>
       <c r="M18" s="33"/>

</xml_diff>

<commit_message>
Se crea la reimpresion de comprobantes
</commit_message>
<xml_diff>
--- a/src/public/plantillas/ReciboDePago.xlsx
+++ b/src/public/plantillas/ReciboDePago.xlsx
@@ -283,6 +283,87 @@
   </si>
   <si>
     <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">N°:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRESCIENTOS SEIS MIL SETECIENTOS NOVENTA Y SEIS PESOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  por:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">N°:63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CERO PESOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin observaciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N°:229</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transf n°:0 | PRUEBA DE EMISION DE COMPROBANTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N°:230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N°:249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CATORCE PESOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N°:167</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NUEVE PESOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">N°:136</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> por:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transferencia a Octano. Número de Operación: 00962142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N°:150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N°:154</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuota4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En concepto de pago en efectivo por Cuota4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N°:155</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuota5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En concepto de pago en efectivo por Cuota5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N°:160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRES PESOS </t>
   </si>
 </sst>
 </file>
@@ -1210,7 +1291,7 @@
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
       <c r="P3" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="Q3"/>
       <c r="S3" s="7"/>
@@ -1285,7 +1366,7 @@
       </c>
       <c r="D8" s="46"/>
       <c r="E8" s="35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F8" s="35"/>
       <c r="G8" s="21"/>
@@ -1344,7 +1425,7 @@
         <v>8</v>
       </c>
       <c r="J11" t="s" s="50">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="K11" s="50"/>
       <c r="L11" s="50"/>
@@ -1423,7 +1504,7 @@
         <v>31</v>
       </c>
       <c r="P15" s="31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q15" s="31"/>
       <c r="R15" s="31"/>
@@ -1471,7 +1552,7 @@
         <v>17</v>
       </c>
       <c r="K18" t="s" s="33">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="L18" s="33"/>
       <c r="M18" s="33"/>

</xml_diff>

<commit_message>
trabajando en pago multiple
</commit_message>
<xml_diff>
--- a/src/public/plantillas/ReciboDePago.xlsx
+++ b/src/public/plantillas/ReciboDePago.xlsx
@@ -145,6 +145,24 @@
   </si>
   <si>
     <t xml:space="preserve">En concepto de pago en efectivo por Cuota2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">N°:214</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 de junio de 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuota1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UN PESO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">En concepto de pago en efectivo por Cuota1</t>
   </si>
   <si>
     <t xml:space="preserve"/>
@@ -1075,7 +1093,7 @@
       <c r="H3" s="39"/>
       <c r="I3" s="39"/>
       <c r="P3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="S3" s="7"/>
     </row>
@@ -1092,7 +1110,7 @@
         <v>11</v>
       </c>
       <c r="N5" t="s" s="21">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="O5" s="21"/>
       <c r="P5" s="21"/>
@@ -1132,7 +1150,7 @@
         <v>6</v>
       </c>
       <c r="L7" t="s" s="26">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="M7" s="26"/>
       <c r="N7" s="26"/>
@@ -1145,11 +1163,11 @@
     <row r="8" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="C8" t="s" s="24">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D8" s="24"/>
       <c r="E8" s="25">
-        <v>6000</v>
+        <v>1</v>
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="40"/>
@@ -1178,7 +1196,7 @@
       <c r="J9" s="30"/>
       <c r="K9" s="30"/>
       <c r="L9" t="s" s="31">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="M9" s="31"/>
       <c r="N9" s="31"/>
@@ -1208,7 +1226,7 @@
         <v>8</v>
       </c>
       <c r="J11" t="s" s="29">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="K11" s="29"/>
       <c r="L11" s="29"/>
@@ -1247,7 +1265,7 @@
       <c r="F13" s="20"/>
       <c r="G13" s="40"/>
       <c r="I13" t="s" s="36">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="J13" s="37"/>
       <c r="K13" s="37"/>
@@ -1287,7 +1305,7 @@
         <v>16</v>
       </c>
       <c r="P15" s="49">
-        <v>6000</v>
+        <v>1</v>
       </c>
       <c r="Q15" s="49"/>
       <c r="R15" s="49"/>
@@ -1335,7 +1353,7 @@
         <v>15</v>
       </c>
       <c r="K18" t="s" s="51">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="L18" s="51"/>
       <c r="M18" s="51"/>

</xml_diff>